<commit_message>
Added - Add address & Save card flow
</commit_message>
<xml_diff>
--- a/app/src/stored-data/dataGenerated.xlsx
+++ b/app/src/stored-data/dataGenerated.xlsx
@@ -2,6 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet name="SignUp Data" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -28,6 +31,191 @@
     </bk>
   </cellMetadata>
 </metadata>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>2026-02-08 09:42:00</t>
+  </si>
+  <si>
+    <t>William Anderson</t>
+  </si>
+  <si>
+    <t>6503885804</t>
+  </si>
+  <si>
+    <t>william12554@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:00:25</t>
+  </si>
+  <si>
+    <t>Kevin Martin</t>
+  </si>
+  <si>
+    <t>2022973898</t>
+  </si>
+  <si>
+    <t>kevin17832@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:05:50</t>
+  </si>
+  <si>
+    <t>Noah Fernandez</t>
+  </si>
+  <si>
+    <t>4152324975</t>
+  </si>
+  <si>
+    <t>noah41581@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:09:07</t>
+  </si>
+  <si>
+    <t>Amanda King</t>
+  </si>
+  <si>
+    <t>6173523882</t>
+  </si>
+  <si>
+    <t>amanda39733@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:25:13</t>
+  </si>
+  <si>
+    <t>Ava Wright</t>
+  </si>
+  <si>
+    <t>6469489000</t>
+  </si>
+  <si>
+    <t>ava5017@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:27:53</t>
+  </si>
+  <si>
+    <t>Sarah Theadore</t>
+  </si>
+  <si>
+    <t>2029648976</t>
+  </si>
+  <si>
+    <t>sarah65649@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:40:39</t>
+  </si>
+  <si>
+    <t>Mark Anderson</t>
+  </si>
+  <si>
+    <t>4159412846</t>
+  </si>
+  <si>
+    <t>mark30403@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:44:13</t>
+  </si>
+  <si>
+    <t>Anna Perez</t>
+  </si>
+  <si>
+    <t>2022629751</t>
+  </si>
+  <si>
+    <t>anna45724@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:48:47</t>
+  </si>
+  <si>
+    <t>Lucas Campbell</t>
+  </si>
+  <si>
+    <t>2019901971</t>
+  </si>
+  <si>
+    <t>lucas18809@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 10:55:30</t>
+  </si>
+  <si>
+    <t>Daniel Turner</t>
+  </si>
+  <si>
+    <t>3053304765</t>
+  </si>
+  <si>
+    <t>daniel21429@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 11:18:39</t>
+  </si>
+  <si>
+    <t>Thomas Nelson</t>
+  </si>
+  <si>
+    <t>6505665339</t>
+  </si>
+  <si>
+    <t>thomas9587@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 11:24:03</t>
+  </si>
+  <si>
+    <t>Chloe Nelson</t>
+  </si>
+  <si>
+    <t>6509016559</t>
+  </si>
+  <si>
+    <t>chloe34996@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 11:32:06</t>
+  </si>
+  <si>
+    <t>Elizabeth Moore</t>
+  </si>
+  <si>
+    <t>3127499466</t>
+  </si>
+  <si>
+    <t>elizabeth18388@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 11:35:44</t>
+  </si>
+  <si>
+    <t>Ryan Phillips</t>
+  </si>
+  <si>
+    <t>6173717907</t>
+  </si>
+  <si>
+    <t>ryan36357@mailinator.com</t>
+  </si>
+  <si>
+    <t>2026-02-08 11:46:05</t>
+  </si>
+  <si>
+    <t>Elizabeth Lewis</t>
+  </si>
+  <si>
+    <t>4157336114</t>
+  </si>
+  <si>
+    <t>elizabeth55251@mailinator.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,79 +585,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" t="str" s="0">
         <v>Timestamp</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" t="str" s="0">
         <v>Full Name</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" t="str" s="0">
         <v>Phone Number</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" t="str" s="0">
         <v>Email</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" t="str" s="0">
         <v>2026-02-08 02:42:39</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" t="str" s="0">
         <v>Lily Martin</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" t="str" s="0">
         <v>9498736462</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" t="str" s="0">
         <v>lily50559@mailinator.com</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" t="str" s="0">
         <v>2026-02-08 02:43:09</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" t="str" s="0">
         <v>Caleb Fernandez</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" t="str" s="0">
         <v>2135764101</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" t="str" s="0">
         <v>caleb80862@mailinator.com</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" t="str" s="0">
         <v>2026-02-08 02:45:05</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" t="str" s="0">
         <v>Amanda Wilson</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" t="str" s="0">
         <v>9498882609</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" t="str" s="0">
         <v>amanda97078@mailinator.com</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" t="str" s="0">
         <v>2026-02-08 02:45:34</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" t="str" s="0">
         <v>Nathan Wright</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" t="str" s="0">
         <v>8185909974</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" t="str" s="0">
         <v>nathan26666@mailinator.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>